<commit_message>
images, about us , add admin table
</commit_message>
<xml_diff>
--- a/public/assets/files/MERIT_LIST.xlsx
+++ b/public/assets/files/MERIT_LIST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Locker\WebD projects\College Level Councelling\Data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7948A4B-AB11-4261-86A4-E716CD41215D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C843A9-0BC1-4D3A-8D5A-195DF7662A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -889,17 +889,17 @@
     <t>44/100</t>
   </si>
   <si>
-    <t>AKSHAY RAWAT</t>
-  </si>
-  <si>
-    <t>ANIL RAWAT</t>
+    <t>RUPESH KUMAR NAMDEV</t>
+  </si>
+  <si>
+    <t>ANKIT NAMDEV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1030,6 +1030,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1376,9 +1383,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1702,13 +1710,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1778,17 +1787,17 @@
       <c r="B2">
         <v>220310141632</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25922</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
         <v>289</v>
-      </c>
-      <c r="D2" s="1">
-        <v>38688</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>290</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>

</xml_diff>